<commit_message>
First analysis of trade shares per region
</commit_message>
<xml_diff>
--- a/data/figure2_countries_regions.xlsx
+++ b/data/figure2_countries_regions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\paper\nature energy\repository\Perspective_Trade\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\paper\normative_trade\repository\Perspective_Trade\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -19,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Area_Source!$A$1:$C$230</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="316">
   <si>
     <t>Aruba</t>
   </si>
@@ -951,6 +951,27 @@
   </si>
   <si>
     <t xml:space="preserve">Central America / Caribbean </t>
+  </si>
+  <si>
+    <t>R5LAM</t>
+  </si>
+  <si>
+    <t>R5OECD90+EU</t>
+  </si>
+  <si>
+    <t>R5REF</t>
+  </si>
+  <si>
+    <t>R5ASIA</t>
+  </si>
+  <si>
+    <t>R5MAF</t>
+  </si>
+  <si>
+    <t>R5ROWO</t>
+  </si>
+  <si>
+    <t>IPCC_1.5D</t>
   </si>
 </sst>
 </file>
@@ -1847,22 +1868,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="4" customWidth="1"/>
-    <col min="2" max="3" width="44.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="58.85546875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="4"/>
+    <col min="1" max="1" width="22.6640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="44.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="58.88671875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>251</v>
       </c>
@@ -1872,14 +1895,18 @@
       <c r="C1" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>229</v>
       </c>
@@ -1890,13 +1917,19 @@
         <v>229</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>231</v>
       </c>
@@ -1907,13 +1940,19 @@
         <v>231</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>37</v>
       </c>
@@ -1924,13 +1963,19 @@
         <v>37</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>298</v>
       </c>
@@ -1940,14 +1985,20 @@
       <c r="C5" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>249</v>
       </c>
@@ -1958,13 +2009,19 @@
         <v>300</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>258</v>
       </c>
@@ -1975,13 +2032,19 @@
         <v>294</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>250</v>
       </c>
@@ -1992,13 +2055,19 @@
         <v>294</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>247</v>
       </c>
@@ -2009,13 +2078,19 @@
         <v>305</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>255</v>
       </c>
@@ -2026,13 +2101,19 @@
         <v>301</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>248</v>
       </c>
@@ -2042,14 +2123,20 @@
       <c r="C11" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
@@ -2060,13 +2147,19 @@
         <v>302</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>291</v>
       </c>
@@ -2077,13 +2170,19 @@
         <v>294</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>52</v>
       </c>
@@ -2094,13 +2193,19 @@
         <v>294</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>297</v>
       </c>
@@ -2110,14 +2215,20 @@
       <c r="C15" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>33</v>
       </c>
@@ -2128,29 +2239,17 @@
         <v>303</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2162,18 +2261,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="41.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>246</v>
       </c>
@@ -2187,7 +2286,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2198,7 +2297,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -2209,7 +2308,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -2220,7 +2319,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2232,7 +2331,7 @@
       </c>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -2243,7 +2342,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -2254,7 +2353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
@@ -2265,7 +2364,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -2276,7 +2375,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -2288,7 +2387,7 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -2299,7 +2398,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -2310,7 +2409,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -2321,7 +2420,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -2332,7 +2431,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -2343,7 +2442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -2354,7 +2453,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -2365,7 +2464,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>63</v>
       </c>
@@ -2376,7 +2475,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -2387,7 +2486,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -2398,7 +2497,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
@@ -2409,7 +2508,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>76</v>
       </c>
@@ -2420,7 +2519,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>77</v>
       </c>
@@ -2431,7 +2530,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>78</v>
       </c>
@@ -2442,7 +2541,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -2453,7 +2552,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>112</v>
       </c>
@@ -2464,7 +2563,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>113</v>
       </c>
@@ -2476,7 +2575,7 @@
       </c>
       <c r="I27" s="15"/>
     </row>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -2488,7 +2587,7 @@
       </c>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>123</v>
       </c>
@@ -2500,7 +2599,7 @@
       </c>
       <c r="I29" s="15"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>126</v>
       </c>
@@ -2511,7 +2610,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>128</v>
       </c>
@@ -2522,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>132</v>
       </c>
@@ -2533,7 +2632,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>135</v>
       </c>
@@ -2544,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>139</v>
       </c>
@@ -2555,7 +2654,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -2566,7 +2665,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>141</v>
       </c>
@@ -2577,7 +2676,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>142</v>
       </c>
@@ -2588,7 +2687,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>145</v>
       </c>
@@ -2600,7 +2699,7 @@
       </c>
       <c r="I38" s="15"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>147</v>
       </c>
@@ -2611,7 +2710,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>148</v>
       </c>
@@ -2622,7 +2721,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>172</v>
       </c>
@@ -2633,7 +2732,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>175</v>
       </c>
@@ -2644,7 +2743,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>176</v>
       </c>
@@ -2655,7 +2754,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>179</v>
       </c>
@@ -2666,7 +2765,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>182</v>
       </c>
@@ -2677,7 +2776,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>184</v>
       </c>
@@ -2688,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>185</v>
       </c>
@@ -2699,7 +2798,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>186</v>
       </c>
@@ -2710,7 +2809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>187</v>
       </c>
@@ -2721,7 +2820,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>192</v>
       </c>
@@ -2736,7 +2835,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>194</v>
       </c>
@@ -2751,7 +2850,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="16"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>197</v>
       </c>
@@ -2762,7 +2861,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>198</v>
       </c>
@@ -2773,7 +2872,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>203</v>
       </c>
@@ -2785,7 +2884,7 @@
       </c>
       <c r="I54" s="15"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>204</v>
       </c>
@@ -2796,7 +2895,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>206</v>
       </c>
@@ -2807,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>208</v>
       </c>
@@ -2818,7 +2917,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>211</v>
       </c>
@@ -2830,7 +2929,7 @@
       </c>
       <c r="F58" s="15"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>212</v>
       </c>
@@ -2841,7 +2940,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>226</v>
       </c>
@@ -2853,7 +2952,7 @@
       </c>
       <c r="F60" s="15"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>227</v>
       </c>
@@ -2865,7 +2964,7 @@
       </c>
       <c r="F61" s="15"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>228</v>
       </c>
@@ -2877,7 +2976,7 @@
       </c>
       <c r="F62" s="15"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
@@ -2888,7 +2987,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>8</v>
       </c>
@@ -2899,7 +2998,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>13</v>
       </c>
@@ -2910,7 +3009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>18</v>
       </c>
@@ -2921,7 +3020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>29</v>
       </c>
@@ -2932,7 +3031,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>30</v>
       </c>
@@ -2943,7 +3042,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
@@ -2955,7 +3054,7 @@
       </c>
       <c r="F69" s="15"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>90</v>
       </c>
@@ -2967,7 +3066,7 @@
       </c>
       <c r="F70" s="15"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>92</v>
       </c>
@@ -2978,7 +3077,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>101</v>
       </c>
@@ -2990,7 +3089,7 @@
       </c>
       <c r="F72" s="15"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>102</v>
       </c>
@@ -3001,7 +3100,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
@@ -3013,7 +3112,7 @@
       </c>
       <c r="F74" s="15"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>105</v>
       </c>
@@ -3025,7 +3124,7 @@
       </c>
       <c r="F75" s="15"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>108</v>
       </c>
@@ -3037,7 +3136,7 @@
       </c>
       <c r="F76" s="15"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>110</v>
       </c>
@@ -3049,7 +3148,7 @@
       </c>
       <c r="F77" s="15"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>116</v>
       </c>
@@ -3060,7 +3159,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>127</v>
       </c>
@@ -3071,7 +3170,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>134</v>
       </c>
@@ -3082,7 +3181,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>137</v>
       </c>
@@ -3093,7 +3192,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>143</v>
       </c>
@@ -3105,7 +3204,7 @@
       </c>
       <c r="F82" s="15"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>152</v>
       </c>
@@ -3116,7 +3215,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>156</v>
       </c>
@@ -3128,7 +3227,7 @@
       </c>
       <c r="F84" s="15"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>159</v>
       </c>
@@ -3139,7 +3238,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>164</v>
       </c>
@@ -3150,7 +3249,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>173</v>
       </c>
@@ -3162,7 +3261,7 @@
       </c>
       <c r="F87" s="14"/>
     </row>
-    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>177</v>
       </c>
@@ -3174,7 +3273,7 @@
       </c>
       <c r="F88" s="14"/>
     </row>
-    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>195</v>
       </c>
@@ -3186,7 +3285,7 @@
       </c>
       <c r="F89" s="14"/>
     </row>
-    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>199</v>
       </c>
@@ -3198,7 +3297,7 @@
       </c>
       <c r="F90" s="14"/>
     </row>
-    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>200</v>
       </c>
@@ -3210,7 +3309,7 @@
       </c>
       <c r="F91" s="14"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>201</v>
       </c>
@@ -3221,7 +3320,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>202</v>
       </c>
@@ -3233,7 +3332,7 @@
       </c>
       <c r="F93" s="14"/>
     </row>
-    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>205</v>
       </c>
@@ -3245,7 +3344,7 @@
       </c>
       <c r="F94" s="14"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>209</v>
       </c>
@@ -3256,7 +3355,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>216</v>
       </c>
@@ -3268,7 +3367,7 @@
       </c>
       <c r="F96" s="14"/>
     </row>
-    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>221</v>
       </c>
@@ -3280,7 +3379,7 @@
       </c>
       <c r="F97" s="14"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>9</v>
       </c>
@@ -3291,7 +3390,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>11</v>
       </c>
@@ -3303,7 +3402,7 @@
       </c>
       <c r="F99" s="14"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>66</v>
       </c>
@@ -3314,7 +3413,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>69</v>
       </c>
@@ -3326,7 +3425,7 @@
       </c>
       <c r="F101" s="14"/>
     </row>
-    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>83</v>
       </c>
@@ -3338,7 +3437,7 @@
       </c>
       <c r="F102" s="14"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -3349,7 +3448,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>130</v>
       </c>
@@ -3361,7 +3460,7 @@
       </c>
       <c r="F104" s="14"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>138</v>
       </c>
@@ -3372,7 +3471,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>146</v>
       </c>
@@ -3384,7 +3483,7 @@
       </c>
       <c r="F106" s="14"/>
     </row>
-    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>153</v>
       </c>
@@ -3396,7 +3495,7 @@
       </c>
       <c r="F107" s="14"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>154</v>
       </c>
@@ -3407,7 +3506,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>160</v>
       </c>
@@ -3418,7 +3517,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>161</v>
       </c>
@@ -3430,7 +3529,7 @@
       </c>
       <c r="F110" s="14"/>
     </row>
-    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>168</v>
       </c>
@@ -3442,7 +3541,7 @@
       </c>
       <c r="F111" s="14"/>
     </row>
-    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>178</v>
       </c>
@@ -3454,7 +3553,7 @@
       </c>
       <c r="F112" s="14"/>
     </row>
-    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>210</v>
       </c>
@@ -3466,7 +3565,7 @@
       </c>
       <c r="F113" s="14"/>
     </row>
-    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>222</v>
       </c>
@@ -3478,7 +3577,7 @@
       </c>
       <c r="F114" s="14"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>223</v>
       </c>
@@ -3489,7 +3588,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>27</v>
       </c>
@@ -3501,7 +3600,7 @@
       </c>
       <c r="F116" s="14"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>37</v>
       </c>
@@ -3513,7 +3612,7 @@
       </c>
       <c r="F117" s="15"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>85</v>
       </c>
@@ -3524,7 +3623,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>121</v>
       </c>
@@ -3535,7 +3634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>4</v>
       </c>
@@ -3546,7 +3645,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>12</v>
       </c>
@@ -3558,7 +3657,7 @@
       </c>
       <c r="F121" s="15"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>15</v>
       </c>
@@ -3569,7 +3668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>19</v>
       </c>
@@ -3581,7 +3680,7 @@
       </c>
       <c r="F123" s="15"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>34</v>
       </c>
@@ -3592,7 +3691,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>50</v>
       </c>
@@ -3604,7 +3703,7 @@
       </c>
       <c r="F125" s="15"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
@@ -3615,7 +3714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>52</v>
       </c>
@@ -3626,7 +3725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>55</v>
       </c>
@@ -3637,7 +3736,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>61</v>
       </c>
@@ -3648,7 +3747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>62</v>
       </c>
@@ -3659,7 +3758,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>64</v>
       </c>
@@ -3670,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>65</v>
       </c>
@@ -3682,7 +3781,7 @@
       </c>
       <c r="F132" s="15"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>67</v>
       </c>
@@ -3693,7 +3792,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>68</v>
       </c>
@@ -3704,7 +3803,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>71</v>
       </c>
@@ -3715,7 +3814,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>74</v>
       </c>
@@ -3726,7 +3825,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>79</v>
       </c>
@@ -3737,7 +3836,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>87</v>
       </c>
@@ -3748,7 +3847,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>89</v>
       </c>
@@ -3760,7 +3859,7 @@
       </c>
       <c r="F139" s="15"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>91</v>
       </c>
@@ -3771,7 +3870,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>93</v>
       </c>
@@ -3782,7 +3881,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>96</v>
       </c>
@@ -3793,7 +3892,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>98</v>
       </c>
@@ -3804,7 +3903,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>115</v>
       </c>
@@ -3816,7 +3915,7 @@
       </c>
       <c r="F144" s="15"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>118</v>
       </c>
@@ -3827,7 +3926,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>119</v>
       </c>
@@ -3838,7 +3937,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>120</v>
       </c>
@@ -3849,7 +3948,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>124</v>
       </c>
@@ -3861,7 +3960,7 @@
       </c>
       <c r="F148" s="15"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>133</v>
       </c>
@@ -3873,7 +3972,7 @@
       </c>
       <c r="F149" s="15"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -3885,7 +3984,7 @@
       </c>
       <c r="F150" s="15"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -3896,7 +3995,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>162</v>
       </c>
@@ -3907,7 +4006,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>165</v>
       </c>
@@ -3918,7 +4017,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>170</v>
       </c>
@@ -3929,7 +4028,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>181</v>
       </c>
@@ -3940,7 +4039,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>189</v>
       </c>
@@ -3952,7 +4051,7 @@
       </c>
       <c r="F156" s="15"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>190</v>
       </c>
@@ -3963,7 +4062,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>191</v>
       </c>
@@ -3974,7 +4073,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>5</v>
       </c>
@@ -3985,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>6</v>
       </c>
@@ -3996,7 +4095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>20</v>
       </c>
@@ -4007,7 +4106,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>94</v>
       </c>
@@ -4018,7 +4117,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>95</v>
       </c>
@@ -4029,7 +4128,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>97</v>
       </c>
@@ -4041,7 +4140,7 @@
       </c>
       <c r="F164" s="15"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>100</v>
       </c>
@@ -4052,7 +4151,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>109</v>
       </c>
@@ -4063,7 +4162,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>111</v>
       </c>
@@ -4074,7 +4173,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>155</v>
       </c>
@@ -4086,7 +4185,7 @@
       </c>
       <c r="F168" s="15"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>167</v>
       </c>
@@ -4097,7 +4196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
@@ -4109,7 +4208,7 @@
       </c>
       <c r="F170" s="15"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>174</v>
       </c>
@@ -4120,7 +4219,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>225</v>
       </c>
@@ -4132,7 +4231,7 @@
       </c>
       <c r="F172" s="15"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +4242,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>10</v>
       </c>
@@ -4154,7 +4253,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>21</v>
       </c>
@@ -4166,7 +4265,7 @@
       </c>
       <c r="F175" s="15"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>24</v>
       </c>
@@ -4177,7 +4276,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>25</v>
       </c>
@@ -4189,7 +4288,7 @@
       </c>
       <c r="F177" s="15"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>28</v>
       </c>
@@ -4200,7 +4299,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>33</v>
       </c>
@@ -4211,7 +4310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>35</v>
       </c>
@@ -4222,7 +4321,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>45</v>
       </c>
@@ -4234,7 +4333,7 @@
       </c>
       <c r="F181" s="15"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>46</v>
       </c>
@@ -4245,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>47</v>
       </c>
@@ -4257,7 +4356,7 @@
       </c>
       <c r="F183" s="15"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>48</v>
       </c>
@@ -4269,7 +4368,7 @@
       </c>
       <c r="F184" s="15"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>49</v>
       </c>
@@ -4281,7 +4380,7 @@
       </c>
       <c r="F185" s="15"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>54</v>
       </c>
@@ -4293,7 +4392,7 @@
       </c>
       <c r="F186" s="15"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>56</v>
       </c>
@@ -4305,7 +4404,7 @@
       </c>
       <c r="F187" s="15"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>80</v>
       </c>
@@ -4317,7 +4416,7 @@
       </c>
       <c r="F188" s="15"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>81</v>
       </c>
@@ -4329,7 +4428,7 @@
       </c>
       <c r="F189" s="15"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>82</v>
       </c>
@@ -4341,7 +4440,7 @@
       </c>
       <c r="F190" s="15"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>88</v>
       </c>
@@ -4353,7 +4452,7 @@
       </c>
       <c r="F191" s="15"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>107</v>
       </c>
@@ -4364,7 +4463,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>114</v>
       </c>
@@ -4376,7 +4475,7 @@
       </c>
       <c r="F193" s="15"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>122</v>
       </c>
@@ -4388,7 +4487,7 @@
       </c>
       <c r="F194" s="15"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>129</v>
       </c>
@@ -4400,7 +4499,7 @@
       </c>
       <c r="F195" s="15"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>144</v>
       </c>
@@ -4412,7 +4511,7 @@
       </c>
       <c r="F196" s="15"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>149</v>
       </c>
@@ -4424,7 +4523,7 @@
       </c>
       <c r="F197" s="15"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>157</v>
       </c>
@@ -4436,7 +4535,7 @@
       </c>
       <c r="F198" s="15"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>163</v>
       </c>
@@ -4448,7 +4547,7 @@
       </c>
       <c r="F199" s="15"/>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>180</v>
       </c>
@@ -4460,7 +4559,7 @@
       </c>
       <c r="F200" s="15"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>193</v>
       </c>
@@ -4472,7 +4571,7 @@
       </c>
       <c r="F201" s="15"/>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>196</v>
       </c>
@@ -4483,7 +4582,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>207</v>
       </c>
@@ -4495,7 +4594,7 @@
       </c>
       <c r="F203" s="14"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>215</v>
       </c>
@@ -4506,7 +4605,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>217</v>
       </c>
@@ -4517,7 +4616,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>219</v>
       </c>
@@ -4528,7 +4627,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>220</v>
       </c>
@@ -4539,7 +4638,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>171</v>
       </c>
@@ -4550,7 +4649,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>7</v>
       </c>
@@ -4561,7 +4660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>26</v>
       </c>
@@ -4572,7 +4671,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>36</v>
       </c>
@@ -4583,7 +4682,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>42</v>
       </c>
@@ -4595,7 +4694,7 @@
       </c>
       <c r="F212" s="14"/>
     </row>
-    <row r="213" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>58</v>
       </c>
@@ -4607,7 +4706,7 @@
       </c>
       <c r="F213" s="14"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>84</v>
       </c>
@@ -4618,7 +4717,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>86</v>
       </c>
@@ -4630,7 +4729,7 @@
       </c>
       <c r="F215" s="14"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>99</v>
       </c>
@@ -4641,7 +4740,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>158</v>
       </c>
@@ -4652,7 +4751,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>166</v>
       </c>
@@ -4663,7 +4762,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>188</v>
       </c>
@@ -4674,7 +4773,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>214</v>
       </c>
@@ -4685,7 +4784,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>218</v>
       </c>
@@ -4696,7 +4795,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>3</v>
       </c>
@@ -4707,7 +4806,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>22</v>
       </c>
@@ -4718,7 +4817,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>23</v>
       </c>
@@ -4729,7 +4828,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>125</v>
       </c>
@@ -4740,7 +4839,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>131</v>
       </c>
@@ -4751,7 +4850,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>136</v>
       </c>
@@ -4762,7 +4861,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>183</v>
       </c>
@@ -4773,7 +4872,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>213</v>
       </c>
@@ -4784,7 +4883,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>224</v>
       </c>
@@ -4809,18 +4908,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2"/>
+    <col min="3" max="3" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>246</v>
       </c>
@@ -4834,7 +4933,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>293</v>
       </c>
@@ -4845,7 +4944,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -4856,7 +4955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>129</v>
       </c>
@@ -4867,7 +4966,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4878,7 +4977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -4889,7 +4988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -4900,7 +4999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -4911,7 +5010,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
@@ -4922,7 +5021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>158</v>
       </c>
@@ -4933,7 +5032,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>235</v>
       </c>
@@ -4945,7 +5044,7 @@
       </c>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>234</v>
       </c>
@@ -4957,7 +5056,7 @@
       </c>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>236</v>
       </c>
@@ -4968,7 +5067,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>282</v>
       </c>
@@ -4979,7 +5078,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>283</v>
       </c>
@@ -4990,7 +5089,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -5001,7 +5100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -5012,7 +5111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -5023,7 +5122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>87</v>
       </c>
@@ -5034,7 +5133,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -5045,7 +5144,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -5056,7 +5155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -5067,7 +5166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -5078,7 +5177,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>65</v>
       </c>
@@ -5089,7 +5188,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
@@ -5100,7 +5199,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -5111,7 +5210,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -5122,7 +5221,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -5133,7 +5232,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>96</v>
       </c>
@@ -5144,7 +5243,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
@@ -5155,7 +5254,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
@@ -5166,7 +5265,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>120</v>
       </c>
@@ -5177,7 +5276,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>118</v>
       </c>
@@ -5188,7 +5287,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>119</v>
       </c>
@@ -5199,7 +5298,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>237</v>
       </c>
@@ -5210,7 +5309,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="36" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>150</v>
       </c>
@@ -5221,7 +5320,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>151</v>
       </c>
@@ -5232,7 +5331,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>162</v>
       </c>
@@ -5243,7 +5342,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>165</v>
       </c>
@@ -5254,7 +5353,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>170</v>
       </c>
@@ -5265,7 +5364,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>232</v>
       </c>
@@ -5276,7 +5375,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>190</v>
       </c>
@@ -5287,7 +5386,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
@@ -5298,7 +5397,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>191</v>
       </c>
@@ -5309,7 +5408,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>34</v>
       </c>
@@ -5320,7 +5419,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>209</v>
       </c>
@@ -5331,7 +5430,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="47" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>71</v>
       </c>
@@ -5342,7 +5441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>284</v>
       </c>
@@ -21733,7 +21832,7 @@
       <c r="XFC48" s="15"/>
       <c r="XFD48" s="15"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
@@ -21744,7 +21843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>23</v>
       </c>
@@ -21755,7 +21854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -21766,7 +21865,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
@@ -21777,7 +21876,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>201</v>
       </c>
@@ -21788,7 +21887,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>213</v>
       </c>
@@ -21799,7 +21898,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>238</v>
       </c>
@@ -21813,7 +21912,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>216</v>
       </c>
@@ -21824,7 +21923,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>285</v>
       </c>
@@ -21835,7 +21934,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>239</v>
       </c>
@@ -21846,7 +21945,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>95</v>
       </c>
@@ -21857,7 +21956,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>97</v>
       </c>
@@ -21868,7 +21967,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>109</v>
       </c>
@@ -21879,7 +21978,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>155</v>
       </c>
@@ -21890,7 +21989,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>169</v>
       </c>
@@ -21901,7 +22000,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>174</v>
       </c>
@@ -21912,7 +22011,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -21923,7 +22022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>286</v>
       </c>
@@ -21934,7 +22033,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>57</v>
       </c>
@@ -21946,7 +22045,7 @@
       </c>
       <c r="G67" s="15"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>230</v>
       </c>
@@ -21957,7 +22056,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>123</v>
       </c>
@@ -21968,7 +22067,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>226</v>
       </c>
@@ -21979,7 +22078,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>240</v>
       </c>
@@ -21990,7 +22089,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>241</v>
       </c>
@@ -22001,7 +22100,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>242</v>
       </c>
@@ -22012,7 +22111,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>288</v>
       </c>
@@ -22023,7 +22122,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>289</v>
       </c>
@@ -22034,7 +22133,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>11</v>
       </c>
@@ -22045,7 +22144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>18</v>
       </c>
@@ -22056,7 +22155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>37</v>
       </c>
@@ -22067,7 +22166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>243</v>
       </c>
@@ -22078,7 +22177,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>92</v>
       </c>
@@ -22090,7 +22189,7 @@
       </c>
       <c r="H80" s="15"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>90</v>
       </c>
@@ -22102,7 +22201,7 @@
       </c>
       <c r="H81" s="15"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>101</v>
       </c>
@@ -22113,7 +22212,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>143</v>
       </c>
@@ -22124,7 +22223,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>154</v>
       </c>
@@ -22135,7 +22234,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>156</v>
       </c>
@@ -22146,7 +22245,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>159</v>
       </c>
@@ -22157,7 +22256,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>177</v>
       </c>
@@ -22168,7 +22267,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>244</v>
       </c>
@@ -22179,7 +22278,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>116</v>
       </c>
@@ -22190,7 +22289,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>245</v>
       </c>
@@ -22201,7 +22300,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>199</v>
       </c>
@@ -22212,7 +22311,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>221</v>
       </c>
@@ -22223,7 +22322,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>287</v>
       </c>

</xml_diff>